<commit_message>
Actualización de los archivos con mejoras de usabilidad
</commit_message>
<xml_diff>
--- a/uploads/1.-FEB-ABRIL 23.xlsx
+++ b/uploads/1.-FEB-ABRIL 23.xlsx
@@ -482,42 +482,42 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PACHUCA DE SOTO</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>HGO</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>817BHK</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>PROCALETI S.C. COLEGIO CERVANTES101 ESCUELA</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>259070801489</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>03 FEB 23 - 04 ABR 23</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>PDBT</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -570,19 +570,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>97466</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>94459</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>3007</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -650,42 +658,42 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2,607.07</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>18.94</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3,631.25</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4,224.84</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>18.64</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>65.90</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>11,095.27</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>528.63</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -748,37 +756,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>65.90</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>554.76</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>11,029.37</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>12,870.51</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1,775.24</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>11,095.27</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>13,425.27</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -793,279 +801,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>IMPORTE</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>KWH</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>PAGOS</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>PERIODO</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>9,366.00</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>9,366.00</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2129</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>05 DIC 22 al 03 FEB 23</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>14,616.00</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>14,616.00</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>3273</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>04 OCT 22 al 05 DIC 22</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>11,121.00</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>11,121.00</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2496</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>03 AGO 22 al 04 OCT 22</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>12,830.00</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>12,830.00</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2901</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>03 JUN 22 al 03 AGO 22</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>8,768.00</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>8,768.00</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>1974</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>05 ABR 22 al 03 JUN 22</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>10,121.00</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>10,121.00</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2352</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>02 FEB 22 al 05 ABR 22</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>6,246.00</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>6,246.00</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1452</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>03 DIC 21 al 02 FEB 22</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>6,010.00</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>6,010.00</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1441</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>04 OCT 21 al 03 DIC 21</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>5,163.00</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>5,163.00</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1239</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>03 AGO 21 al 04 OCT 21</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>4,834.00</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>4,834.00</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1141</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>03 JUN 21 al 03 AGO 21</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>4,205.00</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>4,205.00</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1004</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>05 ABR 21 al 03 JUN 21</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>